<commit_message>
not tested; but percent is 0-1 always
</commit_message>
<xml_diff>
--- a/tests/template/cortex_xlsx_data/00-simple.in/input.xlsx
+++ b/tests/template/cortex_xlsx_data/00-simple.in/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nagler/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C1BF06-F236-AC49-94E2-D27904B9C0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FD5C77-2D51-7B49-8D1E-33C73355A519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -144,9 +144,6 @@
   </si>
   <si>
     <t>structure</t>
-  </si>
-  <si>
-    <t>66%</t>
   </si>
   <si>
     <t>dd</t>
@@ -374,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -391,10 +388,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -407,9 +401,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -424,6 +415,15 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -647,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L986"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -667,35 +667,35 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="16"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="13"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="16">
         <v>3.33</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="13" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
-      <c r="B6" s="21"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="18"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -704,51 +704,51 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="106" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="28" t="s">
+      <c r="C11" s="22"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="12" t="s">
         <v>18</v>
       </c>
       <c r="L12" s="6"/>
@@ -757,59 +757,63 @@
       <c r="A13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12">
-        <v>20</v>
-      </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27">
+        <v>0.2</v>
+      </c>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
       <c r="L13" s="8"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="7">
-        <v>5</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="14">
-        <v>5</v>
-      </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
+      <c r="B14" s="29">
+        <v>0.05</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="30">
+        <v>0.05</v>
+      </c>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7">
-        <v>5</v>
-      </c>
-      <c r="D15" s="14">
-        <v>15</v>
-      </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29">
+        <v>0.05</v>
+      </c>
+      <c r="D15" s="30">
+        <v>0.15</v>
+      </c>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
       <c r="L15" s="8"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="3">
-        <v>65</v>
-      </c>
-      <c r="C16">
-        <v>65</v>
-      </c>
-      <c r="D16" s="3">
-        <v>100</v>
-      </c>
+      <c r="B16" s="31">
+        <v>0.65</v>
+      </c>
+      <c r="C16" s="26">
+        <v>0.65</v>
+      </c>
+      <c r="D16" s="31">
+        <v>1</v>
+      </c>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
     </row>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1796,8 +1800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1817,12 +1821,12 @@
         <v>10</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="20" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1840,7 +1844,7 @@
       <c r="C5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="20" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1852,10 +1856,10 @@
       <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="16" t="s">
+      <c r="B7" s="32">
+        <v>0.66</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2881,7 +2885,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="13" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test passing with 0-100 percents
</commit_message>
<xml_diff>
--- a/tests/template/cortex_xlsx_data/00-simple.in/input.xlsx
+++ b/tests/template/cortex_xlsx_data/00-simple.in/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nagler/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FD5C77-2D51-7B49-8D1E-33C73355A519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E699DDF0-EC07-4A45-A254-C4F828115616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="1280" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
@@ -259,7 +259,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -306,32 +306,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
@@ -371,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -401,13 +375,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -416,15 +390,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L986"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -757,63 +726,63 @@
       <c r="A13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="26"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="27"/>
       <c r="D13" s="27">
-        <v>0.2</v>
-      </c>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
+        <v>20</v>
+      </c>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
       <c r="L13" s="8"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="29">
-        <v>0.05</v>
-      </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="30">
-        <v>0.05</v>
-      </c>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
+      <c r="B14" s="27">
+        <v>5</v>
+      </c>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27">
+        <v>5</v>
+      </c>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29">
-        <v>0.05</v>
-      </c>
-      <c r="D15" s="30">
-        <v>0.15</v>
-      </c>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27">
+        <v>5</v>
+      </c>
+      <c r="D15" s="27">
+        <v>15</v>
+      </c>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
       <c r="L15" s="8"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="31">
-        <v>0.65</v>
-      </c>
-      <c r="C16" s="26">
-        <v>0.65</v>
-      </c>
-      <c r="D16" s="31">
-        <v>1</v>
-      </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
+      <c r="B16" s="27">
+        <v>65</v>
+      </c>
+      <c r="C16" s="27">
+        <v>60</v>
+      </c>
+      <c r="D16" s="27">
+        <v>100</v>
+      </c>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
     </row>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1800,7 +1769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1856,8 +1825,8 @@
       <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="32">
-        <v>0.66</v>
+      <c r="B7" s="26">
+        <v>66</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
nuclides need to be n + z for isotope
</commit_message>
<xml_diff>
--- a/tests/template/cortex_xlsx_data/00-simple.in/input.xlsx
+++ b/tests/template/cortex_xlsx_data/00-simple.in/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nagler/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E699DDF0-EC07-4A45-A254-C4F828115616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92C25B1-F712-6C44-B8A8-E209AE8B045A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1280" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,18 @@
     <sheet name="Operating Conditions" sheetId="2" r:id="rId2"/>
     <sheet name="Geometry" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="oXocW9dz57e8TuhvKhRKNgE/tjePK4A+mdUovBs9kak="/>
     </ext>
@@ -48,9 +58,6 @@
   </si>
   <si>
     <t>Cr</t>
-  </si>
-  <si>
-    <t>W</t>
   </si>
   <si>
     <t>Fe</t>
@@ -147,6 +154,9 @@
   </si>
   <si>
     <t>dd</t>
+  </si>
+  <si>
+    <t>W182</t>
   </si>
 </sst>
 </file>
@@ -375,6 +385,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -390,10 +404,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,7 +627,7 @@
   <dimension ref="A1:L986"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -631,7 +641,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -640,10 +650,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -659,7 +669,7 @@
         <v>3.33</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -673,52 +683,52 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="106" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
+      <c r="A9" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="12" t="s">
+      <c r="E12" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="G12" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="L12" s="6"/>
     </row>
@@ -726,63 +736,63 @@
       <c r="A13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27">
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22">
         <v>20</v>
       </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
       <c r="L13" s="8"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="27">
+      <c r="B14" s="22">
         <v>5</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27">
+      <c r="C14" s="22"/>
+      <c r="D14" s="22">
         <v>5</v>
       </c>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27">
+        <v>39</v>
+      </c>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22">
         <v>5</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="22">
         <v>15</v>
       </c>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
       <c r="L15" s="8"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="27">
+        <v>7</v>
+      </c>
+      <c r="B16" s="22">
         <v>65</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="22">
         <v>60</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="22">
         <v>100</v>
       </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
     </row>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1781,22 +1791,22 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1805,16 +1815,16 @@
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1823,13 +1833,13 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="26">
+        <v>11</v>
+      </c>
+      <c r="B7" s="21">
         <v>66</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2850,43 +2860,43 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>1</v>
@@ -2895,10 +2905,10 @@
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>